<commit_message>
validations: number of attributes
</commit_message>
<xml_diff>
--- a/excel/testing_first_book_into_inventory.xlsx
+++ b/excel/testing_first_book_into_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1990\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{067DE4F2-EA9D-4DF8-A185-BFD166AE6691}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97E2BBFB-5BD0-4321-8F5D-F903EC0FB7D1}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Title</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>ISBN13</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+  </si>
+  <si>
+    <t>exm.jpg</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -427,7 +433,7 @@
     <col min="7" max="7" width="9.14453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +455,11 @@
       <c r="G1" t="s">
         <v>9</v>
       </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -471,6 +480,9 @@
       </c>
       <c r="G2">
         <v>9386000059</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial validation with isbn cases complete
</commit_message>
<xml_diff>
--- a/excel/testing_first_book_into_inventory.xlsx
+++ b/excel/testing_first_book_into_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1990\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97E2BBFB-5BD0-4321-8F5D-F903EC0FB7D1}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68FF876C-8029-4907-8CF6-5E16C1481D12}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -48,9 +48,6 @@
     <t>MRP</t>
   </si>
   <si>
-    <t>arihant indian air force airman group x(English)</t>
-  </si>
-  <si>
     <t>20 practice sets</t>
   </si>
   <si>
@@ -66,19 +63,58 @@
     <t>ISBN13</t>
   </si>
   <si>
-    <t>ImageName</t>
-  </si>
-  <si>
-    <t>exm.jpg</t>
+    <t>supportingImages</t>
+  </si>
+  <si>
+    <t>frontCoverImageName</t>
+  </si>
+  <si>
+    <t>backCoverImageName</t>
+  </si>
+  <si>
+    <t>yearOfPublish</t>
+  </si>
+  <si>
+    <t>NumberOfPages</t>
+  </si>
+  <si>
+    <t>22\03\2004</t>
+  </si>
+  <si>
+    <t>front.jpg</t>
+  </si>
+  <si>
+    <t>back.jpg</t>
+  </si>
+  <si>
+    <t>supporting.jpg</t>
+  </si>
+  <si>
+    <t>nakn</t>
+  </si>
+  <si>
+    <t>nanvdssd</t>
+  </si>
+  <si>
+    <t>085750357X</t>
+  </si>
+  <si>
+    <t>sdsff.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -104,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -420,69 +457,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="9.14453125" customWidth="1"/>
-    <col min="6" max="6" width="11.8359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.14453125" customWidth="1"/>
+    <col min="1" max="1" width="15.87109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.14453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.4375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.4140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.14453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.4921875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6015625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.87109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.64453125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.609375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>140</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9789391464547</v>
+      </c>
+      <c r="G2" s="1">
+        <v>9391464548</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1">
+        <v>300</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
+      <c r="E3" s="1">
+        <v>240</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9788175993105</v>
+      </c>
+      <c r="G3" s="1">
+        <v>8175993103</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1">
+        <v>300</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
         <v>140</v>
       </c>
-      <c r="F2">
-        <v>9789386000057</v>
-      </c>
-      <c r="G2">
-        <v>9386000059</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+      <c r="F4" s="1">
+        <v>9789387022898</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9387022897</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1">
+        <v>90</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9788172343118</v>
+      </c>
+      <c r="G5" s="1">
+        <v>8172343116</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="1">
+        <v>300</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>232</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9788172345198</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8172345194</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1">
+        <v>300</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>140</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9788172344887</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8172344880</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1">
+        <v>300</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>140</v>
+      </c>
+      <c r="F8" s="1">
+        <v>9780857503572</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1">
+        <v>300</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
date of publish is varified
</commit_message>
<xml_diff>
--- a/excel/testing_first_book_into_inventory.xlsx
+++ b/excel/testing_first_book_into_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1990\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68FF876C-8029-4907-8CF6-5E16C1481D12}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02FB7FA4-5C70-4955-84C1-81B7005CC232}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A10" sqref="A10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -747,41 +747,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E10" s="1">
         <v>140</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F10" s="1">
         <v>9780857503572</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K10" s="1">
         <v>300</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
coma separated multiple supportingImages and author complete.
</commit_message>
<xml_diff>
--- a/excel/testing_first_book_into_inventory.xlsx
+++ b/excel/testing_first_book_into_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1990\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACC2ED6F-4D41-4D39-8884-10C863471321}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB3C5C82-84E4-4599-A7B1-C40A63F22942}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>supporting.jpg,supporting.jpg</t>
+  </si>
+  <si>
+    <t>Arihant 'Expert Team', shubham, kinga</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -533,7 +536,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1">
         <v>140</v>

</xml_diff>

<commit_message>
final push No error message included
</commit_message>
<xml_diff>
--- a/excel/testing_first_book_into_inventory.xlsx
+++ b/excel/testing_first_book_into_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1990\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70F3D01F-2C98-4DA3-A18C-055E4AAFEAA8}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52681C10-A190-46EB-ABFD-C59D0949DCE8}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>Title</t>
   </si>
@@ -99,13 +99,13 @@
     <t>085750357X</t>
   </si>
   <si>
-    <t>22\04\2022</t>
-  </si>
-  <si>
     <t>supporting.jpg,supporting.jpg</t>
   </si>
   <si>
     <t>Arihant 'Expert Team', shubham, kinga</t>
+  </si>
+  <si>
+    <t>2\04\2022</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -536,7 +536,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>140</v>
@@ -560,7 +560,7 @@
         <v>300</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
@@ -662,7 +662,7 @@
         <v>8172343116</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
complete date to year correction in yearOfPublish.py
</commit_message>
<xml_diff>
--- a/excel/testing_first_book_into_inventory.xlsx
+++ b/excel/testing_first_book_into_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1990\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52681C10-A190-46EB-ABFD-C59D0949DCE8}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{4D50270A-CFD4-4800-84B0-094C9B389B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E8054F0-3BDD-4812-8605-FC325275C99E}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -63,33 +63,18 @@
     <t>ISBN13</t>
   </si>
   <si>
-    <t>supportingImages</t>
-  </si>
-  <si>
     <t>frontCoverImageName</t>
   </si>
   <si>
-    <t>backCoverImageName</t>
-  </si>
-  <si>
     <t>yearOfPublish</t>
   </si>
   <si>
     <t>NumberOfPages</t>
   </si>
   <si>
-    <t>22\03\2004</t>
-  </si>
-  <si>
     <t>front.jpg</t>
   </si>
   <si>
-    <t>back.jpg</t>
-  </si>
-  <si>
-    <t>supporting.jpg</t>
-  </si>
-  <si>
     <t>nakn</t>
   </si>
   <si>
@@ -99,13 +84,7 @@
     <t>085750357X</t>
   </si>
   <si>
-    <t>supporting.jpg,supporting.jpg</t>
-  </si>
-  <si>
     <t>Arihant 'Expert Team', shubham, kinga</t>
-  </si>
-  <si>
-    <t>2\04\2022</t>
   </si>
 </sst>
 </file>
@@ -463,13 +442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.87109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.14453125" style="1" customWidth="1"/>
@@ -480,14 +459,13 @@
     <col min="7" max="7" width="9.14453125" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.953125" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.4921875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6015625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.87109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.87109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="12.64453125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.609375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,22 +488,16 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -533,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1">
         <v>140</v>
@@ -547,23 +519,17 @@
       <c r="G2" s="1">
         <v>9391464548</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
+      <c r="H2" s="1">
+        <v>2004</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1">
         <v>300</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -585,23 +551,17 @@
       <c r="G3" s="1">
         <v>8175993103</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
+      <c r="H3" s="1">
+        <v>2004</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="1">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1">
         <v>300</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -609,7 +569,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -623,23 +583,17 @@
       <c r="G4" s="1">
         <v>9387022897</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
+      <c r="H4" s="1">
+        <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="1">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1">
         <v>90</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -661,23 +615,17 @@
       <c r="G5" s="1">
         <v>8172343116</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
+      <c r="H5" s="1">
+        <v>20022</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="1">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1">
         <v>300</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -699,23 +647,17 @@
       <c r="G6" s="1">
         <v>8172345194</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
+      <c r="H6" s="1">
+        <v>2034</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="1">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1">
         <v>300</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -737,23 +679,17 @@
       <c r="G7" s="1">
         <v>8172344880</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
+      <c r="H7" s="1">
+        <v>2004</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="1">
+        <v>13</v>
+      </c>
+      <c r="J7" s="1">
         <v>300</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -773,22 +709,16 @@
         <v>9780857503572</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2004</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="1">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1">
         <v>300</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>